<commit_message>
Adding a dictionary explaining the dataset
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louiz\Desktop\data2projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louiz\Desktop\projetRshiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Variable</t>
   </si>
@@ -27,167 +27,209 @@
     <t>Meaning</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Age of the employee</t>
-  </si>
-  <si>
-    <t>Attrition</t>
-  </si>
-  <si>
-    <t>Whether the employee left in the previous year or not</t>
-  </si>
-  <si>
-    <t>BusinessTravel</t>
-  </si>
-  <si>
-    <t>How frequently the employees travelled for business purposes in the last year</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Department in company</t>
-  </si>
-  <si>
-    <t>DistanceFromHome</t>
-  </si>
-  <si>
-    <t>Distance from home in kms</t>
-  </si>
-  <si>
-    <t>Education</t>
-  </si>
-  <si>
-    <t>Education Level</t>
-  </si>
-  <si>
-    <t>EducationField</t>
-  </si>
-  <si>
-    <t>Field of education</t>
-  </si>
-  <si>
-    <t>EnvironmentSatisfaction</t>
-  </si>
-  <si>
-    <t>Work Environment Satisfaction Level</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Gender of employee</t>
-  </si>
-  <si>
-    <t>JobInvolvement</t>
-  </si>
-  <si>
-    <t>Job Involvement Level</t>
-  </si>
-  <si>
-    <t>JobLevel</t>
-  </si>
-  <si>
-    <t>Job level at company on a scale of 1 to 5</t>
-  </si>
-  <si>
-    <t>JobRole</t>
-  </si>
-  <si>
-    <t>Name of job role in company</t>
-  </si>
-  <si>
-    <t>JobSatisfaction</t>
-  </si>
-  <si>
-    <t>Job Satisfaction Level</t>
-  </si>
-  <si>
-    <t>MaritalStatus</t>
-  </si>
-  <si>
-    <t>Marital status of the employee</t>
-  </si>
-  <si>
-    <t>MonthlyIncome</t>
-  </si>
-  <si>
-    <t>Monthly income in rupees per month</t>
-  </si>
-  <si>
-    <t>NumCompaniesWorked</t>
-  </si>
-  <si>
-    <t>Total number of companies the employee has worked for</t>
-  </si>
-  <si>
-    <t>PercentSalaryHike</t>
-  </si>
-  <si>
-    <t>Percent salary hike for last year</t>
-  </si>
-  <si>
-    <t>PerformanceRating</t>
-  </si>
-  <si>
-    <t>Performance rating for last year</t>
-  </si>
-  <si>
-    <t>StandardHours</t>
-  </si>
-  <si>
-    <t>Standard hours of work for the employee</t>
-  </si>
-  <si>
-    <t>StockOptionLevel</t>
-  </si>
-  <si>
-    <t>Stock option level of the employee</t>
-  </si>
-  <si>
-    <t>TotalWorkingYears</t>
-  </si>
-  <si>
-    <t>Total number of years the employee has worked so far</t>
-  </si>
-  <si>
-    <t>TrainingTimesLastYear</t>
-  </si>
-  <si>
-    <t>Number of times training was conducted for this employee last year</t>
-  </si>
-  <si>
-    <t>WorkLifeBalance</t>
-  </si>
-  <si>
-    <t>Work life balance level</t>
-  </si>
-  <si>
-    <t>YearsAtCompany</t>
-  </si>
-  <si>
-    <t>Total number of years spent at the company by the employee</t>
-  </si>
-  <si>
-    <t>YearsSinceLastPromotion</t>
-  </si>
-  <si>
-    <t>Number of years since last promotion</t>
-  </si>
-  <si>
-    <t>YearsWithCurrManager</t>
-  </si>
-  <si>
-    <t>Number of years under current manager</t>
+    <t>school</t>
+  </si>
+  <si>
+    <t>student's school (binary: 'GP' - Gabriel Pereira or 'MS' - Mousinho da Silveira)</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>student's sex (binary: 'F' - female or 'M' - male)</t>
+  </si>
+  <si>
+    <t>age </t>
+  </si>
+  <si>
+    <t>student's age (numeric: from 15 to 22)</t>
+  </si>
+  <si>
+    <t>address </t>
+  </si>
+  <si>
+    <t>student's home address type (binary: 'U' - urban or 'R' - rural)</t>
+  </si>
+  <si>
+    <t>famsize</t>
+  </si>
+  <si>
+    <t>family size (binary: 'LE3' - less or equal to 3 or 'GT3' - greater than 3)</t>
+  </si>
+  <si>
+    <t>Pstatus</t>
+  </si>
+  <si>
+    <t>parent's cohabitation status (binary: 'T' - living together or 'A' - apart)</t>
+  </si>
+  <si>
+    <t>Medu</t>
+  </si>
+  <si>
+    <t>mother's education (numeric: 0 - none, 1 - primary education (4th grade), 2 â€“ 5th to 9th grade, 3 â€“ secondary education or 4 â€“ higher education)</t>
+  </si>
+  <si>
+    <t>Fedu</t>
+  </si>
+  <si>
+    <t>father's education (numeric: 0 - none, 1 - primary education (4th grade), 2 â€“ 5th to 9th grade, 3 â€“ secondary education or 4 â€“ higher education)</t>
+  </si>
+  <si>
+    <t>Mjob</t>
+  </si>
+  <si>
+    <t>mother's job (nominal: 'teacher', 'health' care related, civil 'services' (e.g. administrative or police), 'at_home' or 'other')</t>
+  </si>
+  <si>
+    <t>Fjob</t>
+  </si>
+  <si>
+    <t>father's job (nominal: 'teacher', 'health' care related, civil 'services' (e.g. administrative or police), 'at_home' or 'other')</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>reason to choose this school (nominal: close to 'home', school 'reputation', 'course' preference or 'other')</t>
+  </si>
+  <si>
+    <t>guardian</t>
+  </si>
+  <si>
+    <t>student's guardian (nominal: 'mother', 'father' or 'other')</t>
+  </si>
+  <si>
+    <t>traveltime </t>
+  </si>
+  <si>
+    <t>home to school travel time (numeric: 1 - &lt;15 min., 2 - 15 to 30 min., 3 - 30 min. to 1 hour, or 4 - &gt;1 hour)</t>
+  </si>
+  <si>
+    <t>studytime </t>
+  </si>
+  <si>
+    <t>weekly study time (numeric: 1 - &lt;2 hours, 2 - 2 to 5 hours, 3 - 5 to 10 hours, or 4 - &gt;10 hours)</t>
+  </si>
+  <si>
+    <t>failures</t>
+  </si>
+  <si>
+    <t> number of past class failures (numeric: n if 1&lt;=n&lt;3, else 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schoolsup </t>
+  </si>
+  <si>
+    <t>extra educational support (binary: yes or no)</t>
+  </si>
+  <si>
+    <t>famsup</t>
+  </si>
+  <si>
+    <t> family educational support (binary: yes or no)</t>
+  </si>
+  <si>
+    <t>paid</t>
+  </si>
+  <si>
+    <t>extra paid classes within the course subject (Math or Portuguese) (binary: yes or no)</t>
+  </si>
+  <si>
+    <t>activities</t>
+  </si>
+  <si>
+    <t> extra-curricular activities (binary: yes or no)</t>
+  </si>
+  <si>
+    <t>nursery</t>
+  </si>
+  <si>
+    <t>attended nursery school (binary: yes or no)</t>
+  </si>
+  <si>
+    <t>higher</t>
+  </si>
+  <si>
+    <t>wants to take higher education (binary: yes or no)</t>
+  </si>
+  <si>
+    <t>internet</t>
+  </si>
+  <si>
+    <t>Internet access at home (binary: yes or no)</t>
+  </si>
+  <si>
+    <t>romantic</t>
+  </si>
+  <si>
+    <t>with a romantic relationship (binary: yes or no)</t>
+  </si>
+  <si>
+    <t>famrel</t>
+  </si>
+  <si>
+    <t>quality of family relationships (numeric: from 1 - very bad to 5 - excellent)</t>
+  </si>
+  <si>
+    <t>freetime</t>
+  </si>
+  <si>
+    <t>free time after school (numeric: from 1 - very low to 5 - very high)</t>
+  </si>
+  <si>
+    <t>goout </t>
+  </si>
+  <si>
+    <t>going out with friends (numeric: from 1 - very low to 5 - very high)</t>
+  </si>
+  <si>
+    <t>Dalc</t>
+  </si>
+  <si>
+    <t>workday alcohol consumption (numeric: from 1 - very low to 5 - very high)</t>
+  </si>
+  <si>
+    <t>Walc</t>
+  </si>
+  <si>
+    <t>weekend alcohol consumption (numeric: from 1 - very low to 5 - very high)</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>current health status (numeric: from 1 - very bad to 5 - very good)</t>
+  </si>
+  <si>
+    <t>absences</t>
+  </si>
+  <si>
+    <t>number of school absences (numeric: from 0 to 93)</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>first period grade (numeric: from 0 to 20)</t>
+  </si>
+  <si>
+    <t>G2 </t>
+  </si>
+  <si>
+    <t>second period grade (numeric: from 0 to 20)</t>
+  </si>
+  <si>
+    <t>G3 </t>
+  </si>
+  <si>
+    <t>final grade (numeric: from 0 to 20, output target)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +364,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -510,7 +558,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -640,19 +688,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -702,9 +737,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1060,20 +1093,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="93" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1081,63 +1114,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1145,15 +1178,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1161,23 +1194,23 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -1185,39 +1218,39 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1225,39 +1258,39 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -1265,28 +1298,84 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>